<commit_message>
Fixed button part number
</commit_message>
<xml_diff>
--- a/BOM/xDrip_BOM.xlsx
+++ b/BOM/xDrip_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="465" windowWidth="37155" windowHeight="17340"/>
+    <workbookView xWindow="720" yWindow="468" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="xDrip_BOM" sheetId="1" r:id="rId1"/>
@@ -238,9 +238,6 @@
     <t>C4, C5, C13, C14, C10, C11</t>
   </si>
   <si>
-    <t>311-270JRCT-ND</t>
-  </si>
-  <si>
     <t>587-1227-1-ND</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>160-1434-1-ND</t>
+  </si>
+  <si>
+    <t>CKN10388CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1168,19 +1168,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1194,10 +1194,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1209,10 +1209,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1226,10 +1226,10 @@
         <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1243,10 +1243,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1260,10 +1260,10 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1277,10 +1277,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1294,10 +1294,10 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1311,10 +1311,10 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1328,10 +1328,10 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1345,10 +1345,10 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1362,10 +1362,10 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1379,10 +1379,10 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1396,10 +1396,10 @@
         <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1413,10 +1413,10 @@
         <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1430,10 +1430,10 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1447,10 +1447,10 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1464,10 +1464,10 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1481,10 +1481,10 @@
         <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1498,10 +1498,10 @@
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1515,10 +1515,10 @@
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1532,10 +1532,10 @@
         <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1549,10 +1549,10 @@
         <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1566,10 +1566,10 @@
         <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1583,10 +1583,10 @@
         <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1600,10 +1600,10 @@
         <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1617,10 +1617,10 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1634,10 +1634,10 @@
         <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1651,10 +1651,10 @@
         <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1665,13 +1665,13 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" t="s">
         <v>101</v>
       </c>
-      <c r="E29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1685,10 +1685,10 @@
         <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1702,10 +1702,10 @@
         <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>72</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>